<commit_message>
wait for uni test
</commit_message>
<xml_diff>
--- a/public/data/export/Laporan Peminjaman.xlsx
+++ b/public/data/export/Laporan Peminjaman.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
   <si>
     <t>LAPORAN PEMINJAMAN PERPUSTAKAAN SEKOLAH</t>
   </si>
@@ -56,6 +56,30 @@
     <t>Catatan</t>
   </si>
   <si>
+    <t>siswa satus</t>
+  </si>
+  <si>
+    <t>Testing class</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Buku Paket Bahasa Ingris</t>
+  </si>
+  <si>
+    <t>978-0-393-04002-9</t>
+  </si>
+  <si>
+    <t>26-02-2025</t>
+  </si>
+  <si>
+    <t>25-02-2025</t>
+  </si>
+  <si>
+    <t>Terlambat</t>
+  </si>
+  <si>
     <t>Michael Johnson</t>
   </si>
   <si>
@@ -68,28 +92,7 @@
     <t>978-3-16-148410-0</t>
   </si>
   <si>
-    <t>26-02-2025</t>
-  </si>
-  <si>
     <t>06-03-2025</t>
-  </si>
-  <si>
-    <t>Terlambat</t>
-  </si>
-  <si>
-    <t>siswa satu</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Buku Paket Bahasa Ingris</t>
-  </si>
-  <si>
-    <t>978-0-393-04002-9</t>
-  </si>
-  <si>
-    <t>25-02-2025</t>
   </si>
   <si>
     <t>05-03-2025</t>
@@ -547,18 +550,18 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <pane ySplit="5" activePane="bottomLeft" state="frozen" topLeftCell="A6"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5:M14"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5:M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="5.713" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="18.71" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="9.283" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="16.425" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="12.854" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="29.421" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="21.138" bestFit="true" customWidth="true" style="0"/>
@@ -626,26 +629,26 @@
       <c r="C6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="4">
-        <v>2147483647</v>
+      <c r="D6" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="E6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="4">
         <v>15</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="4">
-        <v>43</v>
-      </c>
       <c r="H6" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
@@ -656,31 +659,31 @@
         <v>2</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="4">
+        <v>2147483647</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="4">
+        <v>43</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="4">
-        <v>15</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
@@ -691,31 +694,31 @@
         <v>3</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D8" s="4">
         <v>2147483647</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G8" s="4">
         <v>24</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
@@ -726,31 +729,31 @@
         <v>4</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D9" s="4">
         <v>2147483647</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G9" s="4">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
@@ -761,31 +764,31 @@
         <v>5</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D10" s="4">
         <v>2147483647</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G10" s="4">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
@@ -796,31 +799,31 @@
         <v>6</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D11" s="4">
         <v>2147483647</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G11" s="4">
         <v>2</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
@@ -831,31 +834,31 @@
         <v>7</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D12" s="4">
         <v>2147483647</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G12" s="4">
         <v>2</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
@@ -871,67 +874,32 @@
       <c r="C13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="4">
-        <v>2147483647</v>
+      <c r="D13" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G13" s="4">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="K13" s="4"/>
+        <v>29</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="4">
-        <v>9</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G14" s="4">
-        <v>21</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
     </row>
   </sheetData>
   <mergeCells>
@@ -946,7 +914,6 @@
     <mergeCell ref="K11:M11"/>
     <mergeCell ref="K12:M12"/>
     <mergeCell ref="K13:M13"/>
-    <mergeCell ref="K14:M14"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>